<commit_message>
refactoring of training code and evaluation results
</commit_message>
<xml_diff>
--- a/evaluation/results/LOF/evaluation_metrics.xlsx
+++ b/evaluation/results/LOF/evaluation_metrics.xlsx
@@ -488,31 +488,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="C2">
-        <v>0.779874213836478</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="D2">
-        <v>0.2066666666666667</v>
+        <v>0.2191011235955056</v>
       </c>
       <c r="E2">
-        <v>0.3267457180500659</v>
+        <v>0.3482142857142857</v>
       </c>
       <c r="F2">
-        <v>0.5705617977528089</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="G2">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="I2">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="J2">
-        <v>476</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -547,13 +547,13 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.5117948717948718</v>
+        <v>0.5516129032258065</v>
       </c>
       <c r="C2">
-        <v>0.9344569288389513</v>
+        <v>0.9606741573033708</v>
       </c>
       <c r="D2">
-        <v>0.6613651424784626</v>
+        <v>0.7008196721311475</v>
       </c>
       <c r="E2">
         <v>534</v>
@@ -564,16 +564,16 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>0.779874213836478</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="C3">
-        <v>0.2066666666666667</v>
+        <v>0.2191011235955056</v>
       </c>
       <c r="D3">
-        <v>0.3267457180500659</v>
+        <v>0.3482142857142857</v>
       </c>
       <c r="E3">
-        <v>600</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -581,16 +581,16 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="C4">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="D4">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="E4">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -598,16 +598,16 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>0.6458345428156749</v>
+        <v>0.699719495091164</v>
       </c>
       <c r="C5">
-        <v>0.570561797752809</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="D5">
-        <v>0.4940554302642642</v>
+        <v>0.5245169789227166</v>
       </c>
       <c r="E5">
-        <v>1134</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -615,16 +615,16 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>0.6536357935100074</v>
+        <v>0.6997194950911642</v>
       </c>
       <c r="C6">
-        <v>0.5493827160493827</v>
+        <v>0.5898876404494382</v>
       </c>
       <c r="D6">
-        <v>0.4843178279660834</v>
+        <v>0.5245169789227166</v>
       </c>
       <c r="E6">
-        <v>1134</v>
+        <v>1068</v>
       </c>
     </row>
   </sheetData>
@@ -653,10 +653,10 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -664,10 +664,10 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>476</v>
+        <v>417</v>
       </c>
       <c r="C3">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>